<commit_message>
Sccoeffs with CIs for all indicators
</commit_message>
<xml_diff>
--- a/2025-04-23/Output/Shift_Indicators/SchematicFigIndicatorScaledCoefficients.xlsx
+++ b/2025-04-23/Output/Shift_Indicators/SchematicFigIndicatorScaledCoefficients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shackelln\Documents\My_Program_Files\R\Hali_Shift_withNF\2025-04-23\Output\Shift_Indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D97C659A-8228-46A9-8833-40C225F9242A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7430816E-E0FE-4766-970E-1E4426531998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>